<commit_message>
Created compact python scripts & User manual
</commit_message>
<xml_diff>
--- a/results/Performance_ClinicalPhenotypes.xlsx
+++ b/results/Performance_ClinicalPhenotypes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Type</t>
   </si>
@@ -22,12 +22,6 @@
     <t>Language</t>
   </si>
   <si>
-    <t>Negation</t>
-  </si>
-  <si>
-    <t>Lemmatizing</t>
-  </si>
-  <si>
     <t>Sensitivy</t>
   </si>
   <si>
@@ -40,48 +34,12 @@
     <t>ClinPhen</t>
   </si>
   <si>
-    <t>heuristic rulebased</t>
-  </si>
-  <si>
     <t>python</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>text2hpo</t>
   </si>
   <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>0.80</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>Monarch</t>
-  </si>
-  <si>
-    <t>java</t>
-  </si>
-  <si>
-    <t>CTAKES</t>
-  </si>
-  <si>
-    <t>MetaMap</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>Neural concept recognizer</t>
   </si>
   <si>
@@ -128,6 +86,15 @@
   </si>
   <si>
     <t>Prior to Entity Linking</t>
+  </si>
+  <si>
+    <t>deep learning</t>
+  </si>
+  <si>
+    <t>rulebased</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -612,8 +579,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -956,449 +925,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A7:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B9">
+        <v>0.65</v>
+      </c>
+      <c r="C9">
+        <v>0.78</v>
+      </c>
+      <c r="D9">
+        <v>0.73</v>
+      </c>
+      <c r="E9">
+        <v>0.72</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>0.96</v>
+      </c>
+      <c r="I9">
+        <v>0.78</v>
+      </c>
+      <c r="J9">
+        <v>0.76</v>
+      </c>
+      <c r="K9">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B10">
+        <v>0.6</v>
+      </c>
+      <c r="C10">
+        <v>0.74</v>
+      </c>
+      <c r="D10">
+        <v>0.7</v>
+      </c>
+      <c r="E10">
+        <v>0.67</v>
+      </c>
+      <c r="G10" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
-        <f>AVERAGE(B17:E17)</f>
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="G2">
-        <f>AVERAGE(B18:E18)</f>
-        <v>0.5675</v>
-      </c>
-      <c r="H2">
-        <f>AVERAGE(B19:E19)</f>
-        <v>0.57250000000000001</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="H10">
+        <v>0.39</v>
+      </c>
+      <c r="I10">
+        <v>0.51</v>
+      </c>
+      <c r="J10">
+        <v>0.63</v>
+      </c>
+      <c r="K10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="s">
+      <c r="B11">
+        <v>0.62</v>
+      </c>
+      <c r="C11">
+        <v>0.76</v>
+      </c>
+      <c r="D11">
+        <v>0.72</v>
+      </c>
+      <c r="E11">
+        <v>0.69</v>
+      </c>
+      <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <f>AVERAGE(B20:E20)</f>
-        <v>0.69000000000000006</v>
-      </c>
-      <c r="G3">
-        <f>AVERAGE(B21:E21)</f>
-        <v>0.58750000000000002</v>
-      </c>
-      <c r="H3">
-        <f>AVERAGE(B22:E22)</f>
-        <v>0.61250000000000004</v>
-      </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="H11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I11">
+        <v>0.62</v>
+      </c>
+      <c r="J11">
+        <v>0.69</v>
+      </c>
+      <c r="K11">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <f>AVERAGE(B14:E14)</f>
+      <c r="B12">
+        <v>0.44</v>
+      </c>
+      <c r="C12" s="1">
         <v>0.72</v>
       </c>
-      <c r="G4">
-        <f>AVERAGE(B15:E15)</f>
-        <v>0.67749999999999999</v>
-      </c>
-      <c r="H4">
-        <f>AVERAGE(B16:E16)</f>
-        <v>0.6974999999999999</v>
-      </c>
-      <c r="J4">
-        <f>AVERAGE(J14:M14)</f>
-        <v>0.77</v>
-      </c>
-      <c r="K4">
-        <f>AVERAGE(J15:M15)</f>
-        <v>0.53249999999999997</v>
-      </c>
-      <c r="L4">
-        <f>AVERAGE(J16:M16)</f>
-        <v>0.61499999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D12">
+        <v>0.59</v>
+      </c>
+      <c r="E12">
+        <v>0.62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>0.81</v>
+      </c>
+      <c r="I12">
+        <v>0.63</v>
+      </c>
+      <c r="J12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K12">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D13">
+        <v>0.64</v>
+      </c>
+      <c r="E13">
+        <v>0.75</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
+        <v>0.37</v>
+      </c>
+      <c r="I13">
+        <v>0.53</v>
+      </c>
+      <c r="J13">
+        <v>0.68</v>
+      </c>
+      <c r="K13">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="D14">
+        <v>0.61</v>
+      </c>
+      <c r="E14">
+        <v>0.68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>0.51</v>
+      </c>
+      <c r="I14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J14">
+        <v>0.61</v>
+      </c>
+      <c r="K14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B15">
+        <v>0.78</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>0.65</v>
+      </c>
+      <c r="E15">
+        <v>0.66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>0.81</v>
+      </c>
+      <c r="I15">
+        <v>0.8</v>
+      </c>
+      <c r="J15">
+        <v>0.65</v>
+      </c>
+      <c r="K15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
-        <v>0.65</v>
-      </c>
-      <c r="C14">
-        <v>0.78</v>
-      </c>
-      <c r="D14">
-        <v>0.73</v>
-      </c>
-      <c r="E14">
-        <v>0.72</v>
-      </c>
-      <c r="I14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14">
-        <v>0.96</v>
-      </c>
-      <c r="K14">
-        <v>0.78</v>
-      </c>
-      <c r="L14">
-        <v>0.76</v>
-      </c>
-      <c r="M14">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-      <c r="C15">
-        <v>0.74</v>
-      </c>
-      <c r="D15">
-        <v>0.7</v>
-      </c>
-      <c r="E15">
-        <v>0.67</v>
-      </c>
-      <c r="I15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15">
-        <v>0.39</v>
-      </c>
-      <c r="K15">
-        <v>0.51</v>
-      </c>
-      <c r="L15">
-        <v>0.63</v>
-      </c>
-      <c r="M15">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
       <c r="B16">
-        <v>0.62</v>
+        <v>0.48</v>
       </c>
       <c r="C16">
-        <v>0.76</v>
+        <v>0.69</v>
       </c>
       <c r="D16">
-        <v>0.72</v>
+        <v>0.69</v>
       </c>
       <c r="E16">
-        <v>0.69</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
+        <v>0.8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>0.44</v>
+      </c>
+      <c r="I16">
+        <v>0.54</v>
       </c>
       <c r="J16">
-        <v>0.56000000000000005</v>
+        <v>0.66</v>
       </c>
       <c r="K16">
-        <v>0.62</v>
-      </c>
-      <c r="L16">
-        <v>0.69</v>
-      </c>
-      <c r="M16">
-        <v>0.59</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>0.81</v>
+        <v>0.59</v>
       </c>
       <c r="C17">
-        <v>0.63</v>
+        <v>0.74</v>
       </c>
       <c r="D17">
-        <v>0.59</v>
+        <v>0.67</v>
       </c>
       <c r="E17">
-        <v>0.51</v>
-      </c>
-      <c r="I17" t="s">
-        <v>30</v>
+        <v>0.72</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I17">
+        <v>0.64</v>
+      </c>
+      <c r="J17">
+        <v>0.66</v>
       </c>
       <c r="K17">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18">
-        <v>0.37</v>
-      </c>
-      <c r="C18">
-        <v>0.53</v>
-      </c>
-      <c r="D18">
-        <v>0.64</v>
-      </c>
-      <c r="E18">
-        <v>0.73</v>
-      </c>
-      <c r="I18" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>0.51</v>
-      </c>
-      <c r="C19">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="D19">
-        <v>0.61</v>
-      </c>
-      <c r="E19">
-        <v>0.6</v>
-      </c>
-      <c r="I19" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19">
-        <v>0.71</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20">
-        <v>0.81</v>
-      </c>
-      <c r="C20">
-        <v>0.8</v>
-      </c>
-      <c r="D20">
-        <v>0.65</v>
-      </c>
-      <c r="E20">
-        <v>0.5</v>
-      </c>
-      <c r="I20" t="s">
-        <v>33</v>
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21">
-        <v>0.44</v>
-      </c>
-      <c r="C21">
-        <v>0.54</v>
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>0.66</v>
+        <f>AVERAGE(B12:K12)</f>
+        <v>0.61</v>
       </c>
       <c r="E21">
-        <v>0.71</v>
-      </c>
-      <c r="I21" t="s">
-        <v>34</v>
+        <f>AVERAGE(B13:K13)</f>
+        <v>0.61874999999999991</v>
+      </c>
+      <c r="F21">
+        <f>AVERAGE(B14:K14)</f>
+        <v>0.59874999999999989</v>
+      </c>
+      <c r="I21">
+        <f>AVERAGE(H12:K12)</f>
+        <v>0.62749999999999995</v>
+      </c>
+      <c r="J21">
+        <f>AVERAGE(H13:K13)</f>
+        <v>0.57750000000000001</v>
+      </c>
+      <c r="K21">
+        <f>AVERAGE(H14:K14)</f>
+        <v>0.57250000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="C22">
-        <v>0.64</v>
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
       </c>
       <c r="D22">
-        <v>0.66</v>
+        <f>AVERAGE(B15:K15)</f>
+        <v>0.70625000000000004</v>
       </c>
       <c r="E22">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
+        <f>AVERAGE(B16:K16)</f>
+        <v>0.62624999999999997</v>
+      </c>
+      <c r="F22">
+        <f>AVERAGE(B17:K17)</f>
+        <v>0.64624999999999999</v>
+      </c>
+      <c r="I22">
+        <f>AVERAGE(H15:K15)</f>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="J22">
+        <f>AVERAGE(H16:K16)</f>
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="K22">
+        <f>AVERAGE(H17:K17)</f>
+        <v>0.61250000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE(B9:E9)</f>
+        <v>0.72</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(B10:E10)</f>
+        <v>0.67749999999999999</v>
+      </c>
+      <c r="F23">
+        <f>AVERAGE(B11:E11)</f>
+        <v>0.6974999999999999</v>
+      </c>
+      <c r="I23">
+        <f>AVERAGE(H9:K9)</f>
+        <v>0.77</v>
+      </c>
+      <c r="J23">
+        <f>AVERAGE(H10:K10)</f>
+        <v>0.53249999999999997</v>
+      </c>
+      <c r="K23">
+        <f>AVERAGE(H11:K11)</f>
+        <v>0.61499999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>